<commit_message>
updated model and fixed fugitive emissions connection
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/brazil/model_input_variables_brazil_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/brazil/model_input_variables_brazil_se_calibrated.xlsx
@@ -603,112 +603,112 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>652.1575389899805</v>
+        <v>2431.942902</v>
       </c>
       <c r="K2">
-        <v>649.4301378089782</v>
+        <v>2421.7722246</v>
       </c>
       <c r="L2">
-        <v>646.7027366279759</v>
+        <v>2411.6015472</v>
       </c>
       <c r="M2">
-        <v>643.9753354469735</v>
+        <v>2401.4308698</v>
       </c>
       <c r="N2">
-        <v>641.2479342659713</v>
+        <v>2391.2601924</v>
       </c>
       <c r="O2">
-        <v>638.520533084969</v>
+        <v>2381.089515</v>
       </c>
       <c r="P2">
-        <v>648.9774607718471</v>
+        <v>2420.084159</v>
       </c>
       <c r="Q2">
-        <v>659.434388458725</v>
+        <v>2459.078803</v>
       </c>
       <c r="R2">
-        <v>669.8913161456032</v>
+        <v>2498.073447</v>
       </c>
       <c r="S2">
-        <v>680.3482438324812</v>
+        <v>2537.068091</v>
       </c>
       <c r="T2">
-        <v>690.8051715193593</v>
+        <v>2576.062735</v>
       </c>
       <c r="U2">
-        <v>709.1737921237219</v>
+        <v>2644.5606574</v>
       </c>
       <c r="V2">
-        <v>727.5424127280846</v>
+        <v>2713.0585798</v>
       </c>
       <c r="W2">
-        <v>745.9110333324472</v>
+        <v>2781.5565022</v>
       </c>
       <c r="X2">
-        <v>764.2796539368098</v>
+        <v>2850.0544246</v>
       </c>
       <c r="Y2">
-        <v>782.6482745411724</v>
+        <v>2918.552347</v>
       </c>
       <c r="Z2">
-        <v>800.2545517972432</v>
+        <v>2984.2074356</v>
       </c>
       <c r="AA2">
-        <v>817.8608290533139</v>
+        <v>3049.8625242</v>
       </c>
       <c r="AB2">
-        <v>835.4671063093845</v>
+        <v>3115.5176128</v>
       </c>
       <c r="AC2">
-        <v>853.0733835654552</v>
+        <v>3181.1727014</v>
       </c>
       <c r="AD2">
-        <v>870.6796608215259</v>
+        <v>3246.82779</v>
       </c>
       <c r="AE2">
-        <v>888.8219116931289</v>
+        <v>3314.4815632</v>
       </c>
       <c r="AF2">
-        <v>906.964162564732</v>
+        <v>3382.1353364</v>
       </c>
       <c r="AG2">
-        <v>925.1064134363349</v>
+        <v>3449.7891096</v>
       </c>
       <c r="AH2">
-        <v>943.248664307938</v>
+        <v>3517.4428828</v>
       </c>
       <c r="AI2">
-        <v>961.3909151795413</v>
+        <v>3585.096656</v>
       </c>
       <c r="AJ2">
-        <v>979.6710077173148</v>
+        <v>3653.2644508</v>
       </c>
       <c r="AK2">
-        <v>997.9511002550884</v>
+        <v>3721.4322456</v>
       </c>
       <c r="AL2">
-        <v>1016.231192792862</v>
+        <v>3789.6000404</v>
       </c>
       <c r="AM2">
-        <v>1034.511285330636</v>
+        <v>3857.7678352</v>
       </c>
       <c r="AN2">
-        <v>1052.79137786841</v>
+        <v>3925.93563</v>
       </c>
       <c r="AO2">
-        <v>1070.805804631178</v>
+        <v>3993.1127378</v>
       </c>
       <c r="AP2">
-        <v>1088.820231393946</v>
+        <v>4060.2898456</v>
       </c>
       <c r="AQ2">
-        <v>1106.834658156714</v>
+        <v>4127.4669534</v>
       </c>
       <c r="AR2">
-        <v>1124.849084919482</v>
+        <v>4194.6440612</v>
       </c>
       <c r="AS2">
-        <v>1142.86351168225</v>
+        <v>4261.821169</v>
       </c>
     </row>
     <row r="3" spans="1:45">
@@ -1335,112 +1335,112 @@
         <v>1</v>
       </c>
       <c r="J8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="K8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="L8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="M8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="N8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="O8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="P8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="Q8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="R8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="S8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="T8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="U8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="V8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="W8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="X8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="Y8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="Z8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AA8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AB8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AC8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AD8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AE8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AF8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AG8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AH8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AI8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AJ8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AK8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AL8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AM8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AN8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AO8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AP8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AQ8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AR8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="AS8">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="9" spans="1:45">
@@ -1457,112 +1457,112 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="Q9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="S9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="T9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="U9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="V9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="W9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="X9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="Y9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="Z9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AA9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AB9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AC9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AD9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AE9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AF9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AG9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AH9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AI9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AK9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AL9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AM9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AN9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AO9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AP9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AQ9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AR9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
       <c r="AS9">
-        <v>1.255730218166831</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:45">
@@ -1945,112 +1945,112 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="K13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="L13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="M13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="N13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="O13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="P13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="Q13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="R13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="S13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="T13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="U13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="V13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="W13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="X13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="Y13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="Z13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AA13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AB13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AC13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AD13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AE13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AF13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AG13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AH13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AI13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AJ13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AK13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AL13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AM13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AN13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AO13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AP13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AQ13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AR13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
       <c r="AS13">
-        <v>4.333861241414868</v>
+        <v>3.145207224</v>
       </c>
     </row>
     <row r="14" spans="1:45">

</xml_diff>